<commit_message>
change index + repository
</commit_message>
<xml_diff>
--- a/ClassByUsed.xlsx
+++ b/ClassByUsed.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Config</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>CustomAuthenticationSuccessHandler.java</t>
+  </si>
+  <si>
+    <t>CommonUtils.java</t>
   </si>
 </sst>
 </file>
@@ -462,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,6 +554,9 @@
       <c r="P3" t="s">
         <v>22</v>
       </c>
+      <c r="R3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">

</xml_diff>